<commit_message>
Fix an issue in REST API.
</commit_message>
<xml_diff>
--- a/resource/TEMPLATE_stock_report.xlsx
+++ b/resource/TEMPLATE_stock_report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15902\go\src\github.com\skeyic\ark-robot\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\COCOA\Hole\ARK\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5458D043-393E-4A34-86AA-A1A5A04B25C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A559654-ACFB-47C3-9E28-85255865ED9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1320" windowWidth="26970" windowHeight="18150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18135" yWindow="3135" windowWidth="22515" windowHeight="19065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>股票</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,8 +47,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -109,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -121,6 +122,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -304,24 +311,30 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>sheet!$B$21:$B$21</c:f>
+              <c:f>sheet!$B$21:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>44284</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sheet!$C$21:$C$21</c:f>
+              <c:f>sheet!$C$21:$C$22</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:formatCode>0_ </c:formatCode>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>10023448</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10002485</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -447,7 +460,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0_ " sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1462,14 +1475,14 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="30.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.625" style="5" customWidth="1"/>
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -1498,7 +1511,7 @@
       <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1509,11 +1522,21 @@
       <c r="B21" s="1">
         <v>44284</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="5">
         <v>10023448</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44285</v>
+      </c>
+      <c r="C22" s="5">
+        <v>10002485</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>